<commit_message>
Genome class unit test completed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -374,84 +374,84 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>111.6192892910541</v>
+        <v>109.2448836041059</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>71.71323905593771</v>
+        <v>74.52689319035321</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -461,27 +461,27 @@
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -489,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="n">
-        <v>0.7911953536668952</v>
+        <v>0.8015459867609394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
population unit tests added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -374,114 +374,114 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>109.2448836041059</v>
+        <v>109.9919950107364</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>74.52689319035321</v>
+        <v>74.44993474229956</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -489,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="n">
-        <v>0.8015459867609394</v>
+        <v>0.7906977336495797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a batch run file that opens the output
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -374,114 +374,114 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>109.9919950107364</v>
+        <v>110.9395668781889</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>74.44993474229956</v>
+        <v>73.37153010941981</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -489,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="n">
-        <v>0.7906977336495797</v>
+        <v>0.7863468976227408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Steel unit test
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -374,114 +374,114 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>110.9395668781889</v>
+        <v>112.9106100093386</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>73.37153010941981</v>
+        <v>68.86544096462683</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -489,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="n">
-        <v>0.7863468976227408</v>
+        <v>0.7981402113560117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added end to end test
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -374,114 +374,114 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>112.9106100093386</v>
+        <v>108.1790132698523</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>68.86544096462683</v>
+        <v>75.52659301172291</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="B13" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="B15" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="B16" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -489,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="n">
-        <v>0.7981402113560117</v>
+        <v>0.8108155531546481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete un-nec excel cells
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Sequence</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>penalty improvement:</t>
+  </si>
+  <si>
+    <t>avg penalty:</t>
   </si>
 </sst>
 </file>
@@ -137,149 +140,260 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>Transition</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>10</c:v>
+                <c:pt idx="39">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$25</c:f>
+              <c:f>Sheet1!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3255</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9856</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.851</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6545</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.21502</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.456</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>8.630000000000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.32</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.12</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>2.156</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>7.45</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.54</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.95</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.538</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.89</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.26</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.26</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.3165</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.235</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.65</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.958</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>6.212</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3255</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.851</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.45</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.538</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.544</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.54</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.456</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.15</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.9856</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.56</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.21502</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.958</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.6</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.6545</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.3165</c:v>
+                <c:pt idx="39">
+                  <c:v>9.449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -381,7 +495,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Zinc Thickness (0.5)</a:t>
+              <a:t>Zinc Thickness (0.2)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -409,149 +523,260 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>Transition</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>10</c:v>
+                <c:pt idx="39">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$25</c:f>
+              <c:f>Sheet1!$C$2:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>73.39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79.15600000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.77</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>74.15600000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>67.15600000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>75.56999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45.2313</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.37</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50.13</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>62.26</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
+                  <c:v>54.89</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55.19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60.36</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>62.15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>74.651651</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43.56</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>61.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>65.05800000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56.91</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64.58</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>69.56100000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>48.38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>78.42400000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>77.54600000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>69.56</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41.76</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>52.25</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>47.874</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>66.114</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>65.15600000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>79.15600000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>78.56</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>74.651651</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>69.56100000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>54.89</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42.15</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43.56</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>45.2313</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>53.15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>52.25</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>40.01</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>50.13</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>67.15600000000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>66.114</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>75.56999999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>74.15600000000001</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>69.56</c:v>
+                <c:pt idx="39">
+                  <c:v>73.69</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>59.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -653,7 +878,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Steel Width (0.2)</a:t>
+              <a:t>Steel Width (0.5)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -681,149 +906,260 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>Transition</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>10</c:v>
+                <c:pt idx="39">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$25</c:f>
+              <c:f>Sheet1!$D$2:$D$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>4.676810340678182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.088681185217801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.102923380843413</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.503907559923784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1561</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.143042986690728</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.456</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.153</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.122999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.456</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.933224351067687</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.456</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>9.9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
+                  <c:v>5.86</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.862212912678877</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.76604421039454</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>5.1651</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>5.478</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.56</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.26684008882887</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.486</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.378241130001514</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.527308460229878</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.56</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.048343367879834</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.320895027321596</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.486357319063728</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.956094143685995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.156000000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.931248289136786</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.56</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.818506109441071</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.46</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>4.78</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.65</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.456</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.478</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.56</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.86</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.56</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.456</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.56</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.1561</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.456</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8.153</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.46</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>8.122999999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.85</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.156000000000001</c:v>
+                <c:pt idx="39">
+                  <c:v>9.008888231495742</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.598283480047998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -953,149 +1289,260 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$25</c:f>
+              <c:f>Sheet1!$A$2:$A$42</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>Transition</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Transition</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>10</c:v>
+                <c:pt idx="39">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$25</c:f>
+              <c:f>Sheet1!$E$2:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>28.49361767952945</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.55001460268919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.94</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65.44450000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.79</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65.2323</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36.69</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>75.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>77.1561651</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74.56</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26.4864</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.80482999499419</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>79.55</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>75.15600000000001</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="17">
+                  <c:v>79.468</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>24.26</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>74.562</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>40.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.54</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28.215145979699</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>53.38472786915824</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23.23</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>40.28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>78.3603</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>44.61120842175305</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>29.24</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>71.76248405286282</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>28.486</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>77.40799787904459</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>64.23</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>26.145</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>65.44450000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>56.56</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>74.562</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>23.23</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>79.468</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65.2323</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>26.4864</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>28.486</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>54.23</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>79.55</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>77.1561651</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>64.23</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>74.56</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>75.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>29.24</c:v>
+                <c:pt idx="39">
+                  <c:v>68.48</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20.285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1591,7 +2038,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1616,378 +2063,711 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B2">
-        <v>8.630000000000001</v>
+        <v>5.45</v>
       </c>
       <c r="C2">
-        <v>62.26</v>
+        <v>73.39</v>
       </c>
       <c r="D2">
-        <v>9.9</v>
+        <v>4.676810340678182</v>
       </c>
       <c r="E2">
-        <v>75.15600000000001</v>
+        <v>28.49361767952945</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
+      <c r="A3">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>8.65</v>
+      </c>
+      <c r="C3">
+        <v>60.28</v>
+      </c>
+      <c r="D3">
+        <v>5.088681185217801</v>
+      </c>
+      <c r="E3">
+        <v>22.55001460268919</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>2.156</v>
+        <v>2.87</v>
       </c>
       <c r="C4">
-        <v>62.15</v>
+        <v>52.436</v>
       </c>
       <c r="D4">
-        <v>5.1651</v>
+        <v>5.102923380843413</v>
       </c>
       <c r="E4">
-        <v>24.26</v>
+        <v>56.94</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>6.212</v>
+        <v>2.3255</v>
       </c>
       <c r="C5">
-        <v>65.15600000000001</v>
+        <v>79.15600000000001</v>
       </c>
       <c r="D5">
-        <v>4.78</v>
+        <v>4.65</v>
       </c>
       <c r="E5">
-        <v>26.145</v>
+        <v>65.44450000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
+      <c r="A6">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.8</v>
+      </c>
+      <c r="C6">
+        <v>43.77</v>
+      </c>
+      <c r="D6">
+        <v>6.503907559923784</v>
+      </c>
+      <c r="E6">
+        <v>56.79</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>2.3255</v>
+        <v>1.9856</v>
       </c>
       <c r="C7">
-        <v>79.15600000000001</v>
+        <v>40.01</v>
       </c>
       <c r="D7">
-        <v>4.65</v>
+        <v>6.1561</v>
       </c>
       <c r="E7">
-        <v>65.44450000000001</v>
+        <v>54.23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>6.851</v>
+        <v>2.544</v>
       </c>
       <c r="C8">
-        <v>78.56</v>
+        <v>42.15</v>
       </c>
       <c r="D8">
-        <v>7.456</v>
+        <v>5.65</v>
       </c>
       <c r="E8">
-        <v>56.56</v>
+        <v>65.2323</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>7.45</v>
+        <v>4.7</v>
       </c>
       <c r="C9">
-        <v>74.651651</v>
+        <v>53.15</v>
       </c>
       <c r="D9">
-        <v>5.478</v>
+        <v>5.75</v>
       </c>
       <c r="E9">
-        <v>74.562</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>9.538</v>
+        <v>6.65</v>
       </c>
       <c r="C10">
-        <v>69.56100000000001</v>
+        <v>61.1</v>
       </c>
       <c r="D10">
-        <v>6.56</v>
+        <v>7.143042986690728</v>
       </c>
       <c r="E10">
-        <v>23.23</v>
+        <v>36.69</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>5</v>
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>6.851</v>
+      </c>
+      <c r="C11">
+        <v>78.56</v>
+      </c>
+      <c r="D11">
+        <v>7.456</v>
+      </c>
+      <c r="E11">
+        <v>56.56</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>8.6</v>
+        <v>2.6545</v>
       </c>
       <c r="C12">
-        <v>54.89</v>
+        <v>74.15600000000001</v>
       </c>
       <c r="D12">
-        <v>5.86</v>
+        <v>9.85</v>
       </c>
       <c r="E12">
-        <v>79.468</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>5</v>
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>4.21502</v>
+      </c>
+      <c r="C13">
+        <v>67.15600000000001</v>
+      </c>
+      <c r="D13">
+        <v>8.153</v>
+      </c>
+      <c r="E13">
+        <v>77.1561651</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>2.544</v>
+        <v>9.6</v>
       </c>
       <c r="C14">
-        <v>42.15</v>
+        <v>75.56999999999999</v>
       </c>
       <c r="D14">
-        <v>5.65</v>
+        <v>8.122999999999999</v>
       </c>
       <c r="E14">
-        <v>65.2323</v>
+        <v>74.56</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>6.54</v>
+        <v>4.456</v>
       </c>
       <c r="C15">
-        <v>43.56</v>
+        <v>45.2313</v>
       </c>
       <c r="D15">
-        <v>4.56</v>
+        <v>7.456</v>
       </c>
       <c r="E15">
-        <v>21</v>
+        <v>26.4864</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B16">
-        <v>4.456</v>
+        <v>3.23</v>
       </c>
       <c r="C16">
-        <v>45.2313</v>
+        <v>48.37</v>
       </c>
       <c r="D16">
-        <v>7.456</v>
+        <v>6.933224351067687</v>
       </c>
       <c r="E16">
-        <v>26.4864</v>
+        <v>48.80482999499419</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>4.7</v>
+        <v>2.56</v>
       </c>
       <c r="C17">
-        <v>53.15</v>
+        <v>50.13</v>
       </c>
       <c r="D17">
-        <v>5.75</v>
+        <v>8.456</v>
       </c>
       <c r="E17">
-        <v>22</v>
+        <v>79.55</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>3.15</v>
+        <v>8.630000000000001</v>
       </c>
       <c r="C18">
-        <v>52.25</v>
+        <v>62.26</v>
       </c>
       <c r="D18">
-        <v>8.56</v>
+        <v>9.9</v>
       </c>
       <c r="E18">
-        <v>28.486</v>
+        <v>75.15600000000001</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>1.9856</v>
+        <v>8.6</v>
       </c>
       <c r="C19">
-        <v>40.01</v>
+        <v>54.89</v>
       </c>
       <c r="D19">
-        <v>6.1561</v>
+        <v>5.86</v>
       </c>
       <c r="E19">
-        <v>54.23</v>
+        <v>79.468</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B20">
-        <v>2.56</v>
+        <v>6.32</v>
       </c>
       <c r="C20">
-        <v>50.13</v>
+        <v>55.19</v>
       </c>
       <c r="D20">
-        <v>8.456</v>
+        <v>6.862212912678877</v>
       </c>
       <c r="E20">
-        <v>79.55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B21">
-        <v>4.21502</v>
+        <v>4.12</v>
       </c>
       <c r="C21">
-        <v>67.15600000000001</v>
+        <v>60.36</v>
       </c>
       <c r="D21">
-        <v>8.153</v>
+        <v>9.76604421039454</v>
       </c>
       <c r="E21">
-        <v>77.1561651</v>
+        <v>54.75</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B22">
-        <v>7.958</v>
+        <v>2.156</v>
       </c>
       <c r="C22">
-        <v>66.114</v>
+        <v>62.15</v>
       </c>
       <c r="D22">
-        <v>7.46</v>
+        <v>5.1651</v>
       </c>
       <c r="E22">
-        <v>64.23</v>
+        <v>24.26</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B23">
-        <v>9.6</v>
+        <v>7.45</v>
       </c>
       <c r="C23">
-        <v>75.56999999999999</v>
+        <v>74.651651</v>
       </c>
       <c r="D23">
-        <v>8.122999999999999</v>
+        <v>5.478</v>
       </c>
       <c r="E23">
-        <v>74.56</v>
+        <v>74.562</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B24">
-        <v>2.6545</v>
+        <v>6.54</v>
       </c>
       <c r="C24">
-        <v>74.15600000000001</v>
+        <v>43.56</v>
       </c>
       <c r="D24">
-        <v>9.85</v>
+        <v>4.56</v>
       </c>
       <c r="E24">
-        <v>75.5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>7.95</v>
+      </c>
+      <c r="C25">
+        <v>61.3</v>
+      </c>
+      <c r="D25">
+        <v>4.26684008882887</v>
+      </c>
+      <c r="E25">
+        <v>40.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>65.05800000000001</v>
+      </c>
+      <c r="D26">
+        <v>4.486</v>
+      </c>
+      <c r="E26">
+        <v>26.54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>7.5</v>
+      </c>
+      <c r="C27">
+        <v>56.91</v>
+      </c>
+      <c r="D27">
+        <v>4.378241130001514</v>
+      </c>
+      <c r="E27">
+        <v>28.215145979699</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>38</v>
+      </c>
+      <c r="B28">
+        <v>9.869999999999999</v>
+      </c>
+      <c r="C28">
+        <v>64.58</v>
+      </c>
+      <c r="D28">
+        <v>6.527308460229878</v>
+      </c>
+      <c r="E28">
+        <v>53.38472786915824</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>9.538</v>
+      </c>
+      <c r="C29">
+        <v>69.56100000000001</v>
+      </c>
+      <c r="D29">
+        <v>6.56</v>
+      </c>
+      <c r="E29">
+        <v>23.23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>5.89</v>
+      </c>
+      <c r="C30">
+        <v>48.38</v>
+      </c>
+      <c r="D30">
+        <v>8.048343367879834</v>
+      </c>
+      <c r="E30">
+        <v>40.28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>0.9</v>
+      </c>
+      <c r="C31">
+        <v>49.6</v>
+      </c>
+      <c r="D31">
+        <v>8.320895027321596</v>
+      </c>
+      <c r="E31">
+        <v>78.3603</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>7.26</v>
+      </c>
+      <c r="C32">
+        <v>78.42400000000001</v>
+      </c>
+      <c r="D32">
+        <v>9.486357319063728</v>
+      </c>
+      <c r="E32">
+        <v>37.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>8.26</v>
+      </c>
+      <c r="C33">
+        <v>77.54600000000001</v>
+      </c>
+      <c r="D33">
+        <v>8.956094143685995</v>
+      </c>
+      <c r="E33">
+        <v>44.61120842175305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
         <v>10</v>
       </c>
-      <c r="B25">
+      <c r="B34">
         <v>2.3165</v>
       </c>
-      <c r="C25">
+      <c r="C34">
         <v>69.56</v>
       </c>
-      <c r="D25">
+      <c r="D34">
         <v>9.156000000000001</v>
       </c>
-      <c r="E25">
+      <c r="E34">
         <v>29.24</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>1.235</v>
+      </c>
+      <c r="C35">
+        <v>41.76</v>
+      </c>
+      <c r="D35">
+        <v>8.931248289136786</v>
+      </c>
+      <c r="E35">
+        <v>71.76248405286282</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>3.15</v>
+      </c>
+      <c r="C36">
+        <v>52.25</v>
+      </c>
+      <c r="D36">
+        <v>8.56</v>
+      </c>
+      <c r="E36">
+        <v>28.486</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>9.65</v>
+      </c>
+      <c r="C37">
+        <v>47.874</v>
+      </c>
+      <c r="D37">
+        <v>6.818506109441071</v>
+      </c>
+      <c r="E37">
+        <v>77.40799787904459</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>7.958</v>
+      </c>
+      <c r="C38">
+        <v>66.114</v>
+      </c>
+      <c r="D38">
+        <v>7.46</v>
+      </c>
+      <c r="E38">
+        <v>64.23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>6.212</v>
+      </c>
+      <c r="C39">
+        <v>65.15600000000001</v>
+      </c>
+      <c r="D39">
+        <v>4.78</v>
+      </c>
+      <c r="E39">
+        <v>26.145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>24</v>
+      </c>
+      <c r="B41">
+        <v>9.449999999999999</v>
+      </c>
+      <c r="C41">
+        <v>73.69</v>
+      </c>
+      <c r="D41">
+        <v>9.008888231495742</v>
+      </c>
+      <c r="E41">
+        <v>68.48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>27</v>
+      </c>
+      <c r="B42">
+        <v>3.2</v>
+      </c>
+      <c r="C42">
+        <v>59.2</v>
+      </c>
+      <c r="D42">
+        <v>7.598283480047998</v>
+      </c>
+      <c r="E42">
+        <v>20.285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
         <v>6</v>
       </c>
-      <c r="B26">
-        <v>0.775169629452419</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
+      <c r="B43">
+        <v>0.7496209143842891</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
         <v>7</v>
       </c>
-      <c r="B27">
-        <v>79.6958948271774</v>
+      <c r="B44">
+        <v>86.31922966216219</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <v>0.2503790856157108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>